<commit_message>
Fix bad smiles in dye2.xlsx
</commit_message>
<xml_diff>
--- a/dye2.xlsx
+++ b/dye2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ykane/w/2006DTX/dye/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ykane/test/PSQ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC37257-C901-6A49-AE93-B96F974D94AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2978A3-AF3B-604E-97DE-31BB037ADA1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5160" yWindow="460" windowWidth="22480" windowHeight="16540" xr2:uid="{5EF17CBE-78AF-F943-9743-36EF1E271D9D}"/>
   </bookViews>
@@ -754,9 +754,6 @@
     <t>CCCCCCCCC1(c2c(c3c1cc(c4sc(c5ccccc5)cc4)cc3)ccc(c(ccc6c7ccccc7)s6(=O)=O)c2)CCCCCCCC</t>
   </si>
   <si>
-    <t>CCCCCCCCC1(c2c(c3c1cc(c(cc4#c5C=CC=C4)s5(=O)=O)cc3)ccc(c(cc6#c7C=CC=C6)s7(=O)=O)c2)CCCCCCCC</t>
-  </si>
-  <si>
     <t>porphyrine</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1055,6 +1052,10 @@
   </si>
   <si>
     <t>53518-19-7</t>
+  </si>
+  <si>
+    <t>CCCCCCCCC1(c2c(c3c1cc(c(cc4c5C=CC=C4)s5(=O)=O)cc3)ccc(c(cc6c7C=CC=C6)s7(=O)=O)c2)CCCCCCCC</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -1551,8 +1552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7EF596F-29EA-9A4A-A612-FF8860B68144}">
   <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106:XFD106"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E60" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -1578,13 +1579,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G1" t="s">
         <v>15</v>
       </c>
       <c r="H1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1604,7 +1605,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G2">
         <v>3</v>
@@ -1624,7 +1625,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1647,7 +1648,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -1670,7 +1671,7 @@
         <v>25</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G5">
         <v>3</v>
@@ -1693,7 +1694,7 @@
         <v>26</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -1716,7 +1717,7 @@
         <v>20</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G7">
         <v>3</v>
@@ -1724,7 +1725,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B8" t="s">
         <v>44</v>
@@ -1736,10 +1737,10 @@
         <v>5.7000000000000002E-3</v>
       </c>
       <c r="E8" t="s">
+        <v>254</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>255</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>256</v>
       </c>
       <c r="G8">
         <v>8</v>
@@ -1762,7 +1763,7 @@
         <v>71</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G9">
         <v>8</v>
@@ -1770,7 +1771,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B10" t="s">
         <v>44</v>
@@ -1785,7 +1786,7 @@
         <v>73</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G10">
         <v>8</v>
@@ -1793,7 +1794,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B11" t="s">
         <v>44</v>
@@ -1805,10 +1806,10 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>262</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>263</v>
       </c>
       <c r="G11">
         <v>8</v>
@@ -1831,7 +1832,7 @@
         <v>75</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G12">
         <v>8</v>
@@ -1854,7 +1855,7 @@
         <v>83</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G13">
         <v>8</v>
@@ -1877,7 +1878,7 @@
         <v>85</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G14">
         <v>8</v>
@@ -1900,7 +1901,7 @@
         <v>88</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G15">
         <v>8</v>
@@ -1908,7 +1909,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B16" t="s">
         <v>44</v>
@@ -1920,10 +1921,10 @@
         <v>0.02</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G16">
         <v>8</v>
@@ -1946,7 +1947,7 @@
         <v>76</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G17">
         <v>8</v>
@@ -1954,7 +1955,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B18" t="s">
         <v>44</v>
@@ -1969,7 +1970,7 @@
         <v>78</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G18">
         <v>8</v>
@@ -1977,7 +1978,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B19" t="s">
         <v>44</v>
@@ -1992,7 +1993,7 @@
         <v>79</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G19">
         <v>8</v>
@@ -2015,7 +2016,7 @@
         <v>89</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G20">
         <v>8</v>
@@ -2038,7 +2039,7 @@
         <v>94</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G21">
         <v>8</v>
@@ -2061,7 +2062,7 @@
         <v>7</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G22">
         <v>8</v>
@@ -2081,7 +2082,7 @@
         <v>181</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G23">
         <v>10</v>
@@ -2104,7 +2105,7 @@
         <v>175</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G24">
         <v>8</v>
@@ -2124,7 +2125,7 @@
         <v>193</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G25">
         <v>10</v>
@@ -2147,18 +2148,18 @@
         <v>27</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G26">
         <v>4</v>
       </c>
       <c r="H26" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B27" t="s">
         <v>44</v>
@@ -2312,7 +2313,7 @@
         <v>50</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G35">
         <v>4</v>
@@ -2363,7 +2364,7 @@
         <v>0.71</v>
       </c>
       <c r="E38" t="s">
-        <v>202</v>
+        <v>291</v>
       </c>
       <c r="G38">
         <v>11</v>
@@ -2470,7 +2471,7 @@
         <v>69</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G44">
         <v>8</v>
@@ -2487,7 +2488,7 @@
         <v>0.67</v>
       </c>
       <c r="E45" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G45">
         <v>8</v>
@@ -2525,13 +2526,13 @@
         <v>0.63</v>
       </c>
       <c r="E47" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G47">
         <v>8</v>
       </c>
       <c r="I47" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -2545,7 +2546,7 @@
         <v>0.62</v>
       </c>
       <c r="E48" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G48">
         <v>11</v>
@@ -2568,13 +2569,13 @@
         <v>30</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G49">
         <v>4</v>
       </c>
       <c r="H49" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2594,13 +2595,13 @@
         <v>31</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G50">
         <v>4</v>
       </c>
       <c r="H50" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="21">
@@ -2620,7 +2621,7 @@
         <v>52</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G51">
         <v>4</v>
@@ -2679,18 +2680,18 @@
         <v>96</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G54">
         <v>15</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B55" t="s">
         <v>44</v>
@@ -2702,10 +2703,10 @@
         <v>0.09</v>
       </c>
       <c r="E55" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F55" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>288</v>
       </c>
       <c r="G55">
         <v>15</v>
@@ -2714,7 +2715,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B56" t="s">
         <v>44</v>
@@ -2726,10 +2727,10 @@
         <v>0.8</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G56">
         <v>15</v>
@@ -2807,13 +2808,13 @@
         <v>53</v>
       </c>
       <c r="F60" s="15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G60">
         <v>4</v>
       </c>
       <c r="H60" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2827,7 +2828,7 @@
         <v>0.4</v>
       </c>
       <c r="E61" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G61">
         <v>11</v>
@@ -2901,7 +2902,7 @@
         <v>149</v>
       </c>
       <c r="F65" s="15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G65">
         <v>4</v>
@@ -2978,13 +2979,13 @@
         <v>54</v>
       </c>
       <c r="F69" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G69">
         <v>4</v>
       </c>
       <c r="H69" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -3001,16 +3002,16 @@
         <v>0.16</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F70" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G70">
         <v>4</v>
       </c>
       <c r="H70" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -3030,7 +3031,7 @@
         <v>47</v>
       </c>
       <c r="F71" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G71">
         <v>4</v>
@@ -3053,13 +3054,13 @@
         <v>51</v>
       </c>
       <c r="F72" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G72">
         <v>4</v>
       </c>
       <c r="H72" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -3079,7 +3080,7 @@
         <v>150</v>
       </c>
       <c r="F73" s="15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G73">
         <v>4</v>
@@ -3279,7 +3280,7 @@
         <v>56</v>
       </c>
       <c r="F84" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G84">
         <v>4</v>
@@ -3287,7 +3288,7 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B85" t="s">
         <v>44</v>
@@ -3319,7 +3320,7 @@
         <v>57</v>
       </c>
       <c r="F86" s="15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G86">
         <v>4</v>
@@ -3342,7 +3343,7 @@
         <v>59</v>
       </c>
       <c r="F87" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G87">
         <v>4</v>
@@ -3394,7 +3395,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F90" s="11"/>
       <c r="G90">
@@ -3412,7 +3413,7 @@
         <v>1E-3</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F91" s="11"/>
       <c r="G91">
@@ -3478,7 +3479,7 @@
         <v>1</v>
       </c>
       <c r="F94" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G94">
         <v>1</v>
@@ -3524,7 +3525,7 @@
     </row>
     <row r="97" spans="1:7">
       <c r="A97" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B97" t="s">
         <v>6</v>
@@ -3533,10 +3534,10 @@
         <v>0.99</v>
       </c>
       <c r="E97" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F97" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G97">
         <v>12</v>
@@ -3552,7 +3553,7 @@
     </row>
     <row r="99" spans="1:7">
       <c r="A99" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B99" t="s">
         <v>6</v>
@@ -3561,10 +3562,10 @@
         <v>0.6</v>
       </c>
       <c r="E99" t="s">
+        <v>215</v>
+      </c>
+      <c r="F99" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="F99" s="11" t="s">
-        <v>217</v>
       </c>
       <c r="G99">
         <v>13</v>
@@ -3572,7 +3573,7 @@
     </row>
     <row r="100" spans="1:7">
       <c r="A100" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B100" t="s">
         <v>6</v>
@@ -3581,7 +3582,7 @@
         <v>0.83</v>
       </c>
       <c r="E100" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G100">
         <v>14</v>
@@ -3589,7 +3590,7 @@
     </row>
     <row r="101" spans="1:7">
       <c r="A101" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B101" t="s">
         <v>6</v>
@@ -3601,10 +3602,10 @@
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="E101" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F101" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G101">
         <v>8</v>
@@ -3612,7 +3613,7 @@
     </row>
     <row r="102" spans="1:7">
       <c r="A102" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B102" t="s">
         <v>6</v>
@@ -3624,10 +3625,10 @@
         <v>0.97</v>
       </c>
       <c r="E102" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F102" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G102">
         <v>8</v>
@@ -3650,7 +3651,7 @@
         <v>96</v>
       </c>
       <c r="F103" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G103">
         <v>15</v>
@@ -3658,7 +3659,7 @@
     </row>
     <row r="104" spans="1:7">
       <c r="A104" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B104" t="s">
         <v>6</v>
@@ -3670,10 +3671,10 @@
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="E104" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F104" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>288</v>
       </c>
       <c r="G104">
         <v>15</v>
@@ -3696,7 +3697,7 @@
         <v>96</v>
       </c>
       <c r="F105" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G105">
         <v>15</v>
@@ -3704,7 +3705,7 @@
     </row>
     <row r="106" spans="1:7">
       <c r="A106" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B106" t="s">
         <v>14</v>
@@ -3716,10 +3717,10 @@
         <v>0.98</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G106">
         <v>15</v>
@@ -3853,7 +3854,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -3861,7 +3862,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -3869,7 +3870,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -3877,7 +3878,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="16" spans="1:20">

</xml_diff>